<commit_message>
fixing an issue odextend.m
Made sure that the second numerical integration is working as intended.

-Removed unnecessary if-statement from the cumulative mole event for adsorber 1 at the product end.

-added getExTaEventMoleFracCum.m, which was missing
</commit_message>
<xml_diff>
--- a/6_publication/1_toPSAil/2_data/3.0_computational_benefits_comparisons/comparisons_num_eff_2023_01_01_v1.xlsx
+++ b/6_publication/1_toPSAil/2_data/3.0_computational_benefits_comparisons/comparisons_num_eff_2023_01_01_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tkim333\Documents\GitHub\toPSAil\6_publication\1_toPSAil\2_data\3.0_computational_benefits_comparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D10F18-539F-4F2B-9B96-7FD785265A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907D3946-B588-4B7C-84EB-E91512D50716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{629B569E-946E-4B1C-9D49-8264BBEF7928}"/>
   </bookViews>
@@ -320,272 +320,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{E1CF349A-851F-43A8-84EB-DE139FF81E68}"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -898,7 +633,7 @@
   <dimension ref="A3:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="K4" sqref="K4:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1000,28 +735,28 @@
         <f>H4/I4</f>
         <v>0.1013750720471881</v>
       </c>
-      <c r="K4" s="7">
-        <v>426.42200000000003</v>
-      </c>
-      <c r="L4" s="7">
-        <v>444.43799999999999</v>
-      </c>
-      <c r="M4" s="7">
-        <v>411.92200000000003</v>
-      </c>
-      <c r="N4" s="7">
-        <v>413.04700000000003</v>
-      </c>
-      <c r="O4" s="7">
-        <v>421.14100000000002</v>
+      <c r="K4" s="1">
+        <v>400.18799999999999</v>
+      </c>
+      <c r="L4" s="1">
+        <v>413.70299999999997</v>
+      </c>
+      <c r="M4" s="1">
+        <v>399.68799999999999</v>
+      </c>
+      <c r="N4" s="1">
+        <v>385.375</v>
+      </c>
+      <c r="O4" s="1">
+        <v>395.03100000000001</v>
       </c>
       <c r="P4" s="8">
         <f>AVERAGE(K4:O4)/G4</f>
-        <v>70.565666666666672</v>
+        <v>66.466166666666666</v>
       </c>
       <c r="Q4" s="9">
         <f>P4/E4</f>
-        <v>35.282833333333336</v>
+        <v>33.233083333333333</v>
       </c>
     </row>
     <row r="5" spans="1:17">

</xml_diff>